<commit_message>
making sure inputs are up to date
</commit_message>
<xml_diff>
--- a/kep2groupscatterinput.xlsx
+++ b/kep2groupscatterinput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aiden\Documents\Python\NPRE247\ComputerProject2Kepford\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A1BEEF-9390-4508-BE48-5844DBD3B234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77ABE495-6560-4E2C-B684-64DF02A80A12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1608" yWindow="1908" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>scatter1</t>
+  </si>
+  <si>
+    <t>scatter2</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -350,11 +357,11 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>